<commit_message>
Updated Self Execution set
</commit_message>
<xml_diff>
--- a/Projects/INBEVTRADMX_SAND/Data/inbevtradmx_template_4_v2.xlsx
+++ b/Projects/INBEVTRADMX_SAND/Data/inbevtradmx_template_4_v2.xlsx
@@ -539,7 +539,7 @@
     <t xml:space="preserve">Hay o no hay # frentes</t>
   </si>
   <si>
-    <t xml:space="preserve">Michelob Ultra</t>
+    <t xml:space="preserve">Michelob</t>
   </si>
   <si>
     <t xml:space="preserve">Product Availability KPI: If in scene type "Exhibicion Especial" there is at least 20 facings from the same brand_name from ABI-GM manufacturer, then pass.</t>
@@ -958,17 +958,20 @@
   </sheetPr>
   <dimension ref="A1:U65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R35" activeCellId="0" sqref="R35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M53" activeCellId="0" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="55.8877551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.765306122449"/>
+    <col collapsed="false" hidden="false" max="19" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="55.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4057,6 +4060,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
@@ -4181,6 +4187,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4204,6 +4213,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4248,6 +4260,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
Modified Set Self Execution to reflect changes in PROS ticket
</commit_message>
<xml_diff>
--- a/Projects/INBEVTRADMX_SAND/Data/inbevtradmx_template_4_v2.xlsx
+++ b/Projects/INBEVTRADMX_SAND/Data/inbevtradmx_template_4_v2.xlsx
@@ -539,7 +539,7 @@
     <t xml:space="preserve">Hay o no hay # frentes</t>
   </si>
   <si>
-    <t xml:space="preserve">Michelob</t>
+    <t xml:space="preserve">Budlight</t>
   </si>
   <si>
     <t xml:space="preserve">Product Availability KPI: If in scene type "Exhibicion Especial" there is at least 20 facings from the same brand_name from ABI-GM manufacturer, then pass.</t>
@@ -959,19 +959,19 @@
   <dimension ref="A1:U65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M53" activeCellId="0" sqref="M53"/>
+      <selection pane="topLeft" activeCell="T38" activeCellId="0" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.765306122449"/>
-    <col collapsed="false" hidden="false" max="19" min="7" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="55.2091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2295918367347"/>
+    <col collapsed="false" hidden="false" max="19" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="54.5357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4061,7 +4061,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4188,7 +4188,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4214,7 +4214,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4261,7 +4261,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>